<commit_message>
Se avanzo en el generar excel
</commit_message>
<xml_diff>
--- a/parqueadero-service/reporte.xlsx
+++ b/parqueadero-service/reporte.xlsx
@@ -7,40 +7,68 @@
   </bookViews>
   <sheets>
     <sheet name="Parqueados Primera Vez" r:id="rId3" sheetId="1"/>
-    <sheet name="Mas Registrados Diferentes Parq" r:id="rId4" sheetId="2"/>
-    <sheet name="Mas Registrados en un parqueade" r:id="rId5" sheetId="3"/>
+    <sheet name="Vehiculos más registrados (D.P)" r:id="rId4" sheetId="2"/>
+    <sheet name="Vehiculos más registrados en P" r:id="rId5" sheetId="3"/>
     <sheet name="Ganancias de un parqueadero" r:id="rId6" sheetId="4"/>
+    <sheet name="Coincidencias de placa" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Vehículos Parqueados por Primera Vez</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Placa</t>
+  </si>
+  <si>
+    <t>Fecha de Ingreso</t>
+  </si>
+  <si>
+    <t>DXL705</t>
+  </si>
+  <si>
+    <t>2024-03-17 16:09:29</t>
+  </si>
+  <si>
+    <t>DCO657</t>
+  </si>
+  <si>
+    <t>2024-03-17 16:09:38</t>
+  </si>
+  <si>
+    <t>DPO896</t>
+  </si>
+  <si>
+    <t>2024-03-17 16:09:43</t>
+  </si>
+  <si>
     <t>Vehículos más veces registrados en diferentes parqueaderos</t>
   </si>
   <si>
-    <t>Vehículos más veces registrados en un parqueadero: Parqueadero Barato</t>
-  </si>
-  <si>
-    <t>Ganancias de un parqueadero: Parqueadero Barato</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Placa</t>
-  </si>
-  <si>
-    <t>Fecha de Ingreso</t>
-  </si>
-  <si>
     <t>Cantidad veces registrado</t>
   </si>
   <si>
+    <t>DML343</t>
+  </si>
+  <si>
+    <t>DX4A20</t>
+  </si>
+  <si>
+    <t>DMY700</t>
+  </si>
+  <si>
+    <t>DML777</t>
+  </si>
+  <si>
+    <t>Vehículos más veces registrados en un parqueadero: Parqueadero Barato XL</t>
+  </si>
+  <si>
     <t>Hoy</t>
   </si>
   <si>
@@ -53,70 +81,22 @@
     <t>Año</t>
   </si>
   <si>
-    <t>KLA453</t>
-  </si>
-  <si>
-    <t>2024-02-28 09:31:17</t>
-  </si>
-  <si>
-    <t>KLA488</t>
-  </si>
-  <si>
-    <t>2024-02-28 09:38:20</t>
-  </si>
-  <si>
-    <t>KLZ976</t>
-  </si>
-  <si>
-    <t>2024-02-28 09:39:24</t>
-  </si>
-  <si>
-    <t>KLY278</t>
-  </si>
-  <si>
-    <t>2024-02-28 09:42:04</t>
-  </si>
-  <si>
-    <t>MIK782</t>
-  </si>
-  <si>
-    <t>KLS878</t>
-  </si>
-  <si>
-    <t>ULM349</t>
-  </si>
-  <si>
-    <t>UML777</t>
-  </si>
-  <si>
-    <t>XML343</t>
-  </si>
-  <si>
-    <t>DML343</t>
-  </si>
-  <si>
-    <t>DML777</t>
-  </si>
-  <si>
-    <t>ZAP234</t>
-  </si>
-  <si>
-    <t>DMM974</t>
-  </si>
-  <si>
-    <t>DMR978</t>
-  </si>
-  <si>
-    <t>Las ganancias de la fecha de hoy 2024-03-15 son: $ 0</t>
-  </si>
-  <si>
-    <t>Las ganancias de esta semana son: $ 0</t>
-  </si>
-  <si>
-    <t>Las ganancias del mes de MARCH son: $ 0</t>
-  </si>
-  <si>
-    <t>Las ganancias del año de 2024 son: $ 27.950</t>
+    <t>Ganancias de un parqueadero: Parqueadero Barato XL</t>
+  </si>
+  <si>
+    <t>Las ganancias de la fecha de hoy 2024-03-17 son: $ 6.400</t>
+  </si>
+  <si>
+    <t>Las ganancias de esta semana son: $ 6.400</t>
+  </si>
+  <si>
+    <t>Las ganancias del mes de MARCH son: $ 6.400</t>
+  </si>
+  <si>
+    <t>Las ganancias del año de 2024 son: $ 6.400</t>
+  </si>
+  <si>
+    <t>Coincidencias de la placa: D</t>
   </si>
 </sst>
 </file>
@@ -224,7 +204,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -237,57 +217,46 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>18.0</v>
+        <v>5.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>19.0</v>
+        <v>6.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>20.0</v>
+        <v>7.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -300,7 +269,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -308,127 +277,94 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>30.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>29.0</v>
+        <v>4.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>12.0</v>
+        <v>7.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="3" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -442,7 +378,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,29 +386,29 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>29.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +416,7 @@
         <v>4.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>2.0</v>
@@ -488,10 +424,10 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>1.0</v>
@@ -499,10 +435,10 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>18.0</v>
+        <v>1.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>1.0</v>
@@ -510,10 +446,10 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>21.0</v>
+        <v>5.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>1.0</v>
@@ -521,10 +457,10 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>19.0</v>
+        <v>6.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>1.0</v>
@@ -532,23 +468,12 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>20.0</v>
+        <v>7.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -562,7 +487,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -570,21 +495,89 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se implementó lo de asincrono, doble paralelo y tarea asincrona
</commit_message>
<xml_diff>
--- a/parqueadero-service/reporte.xlsx
+++ b/parqueadero-service/reporte.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Vehículos Parqueados por Primera Vez</t>
   </si>
@@ -30,22 +30,28 @@
     <t>Fecha de Ingreso</t>
   </si>
   <si>
-    <t>DXL705</t>
-  </si>
-  <si>
-    <t>2024-03-17 16:09:29</t>
-  </si>
-  <si>
-    <t>DCO657</t>
-  </si>
-  <si>
-    <t>2024-03-17 16:09:38</t>
-  </si>
-  <si>
-    <t>DPO896</t>
-  </si>
-  <si>
-    <t>2024-03-17 16:09:43</t>
+    <t>ULM345</t>
+  </si>
+  <si>
+    <t>2024-02-27 12:43:53</t>
+  </si>
+  <si>
+    <t>DML349</t>
+  </si>
+  <si>
+    <t>2024-02-27 15:12:38</t>
+  </si>
+  <si>
+    <t>DMM974</t>
+  </si>
+  <si>
+    <t>2024-02-27 15:51:41</t>
+  </si>
+  <si>
+    <t>DMR978</t>
+  </si>
+  <si>
+    <t>2024-02-27 15:51:53</t>
   </si>
   <si>
     <t>Vehículos más veces registrados en diferentes parqueaderos</t>
@@ -54,19 +60,31 @@
     <t>Cantidad veces registrado</t>
   </si>
   <si>
+    <t>MIK782</t>
+  </si>
+  <si>
+    <t>KLS878</t>
+  </si>
+  <si>
+    <t>ULM349</t>
+  </si>
+  <si>
+    <t>UML777</t>
+  </si>
+  <si>
+    <t>XML343</t>
+  </si>
+  <si>
     <t>DML343</t>
   </si>
   <si>
-    <t>DX4A20</t>
-  </si>
-  <si>
-    <t>DMY700</t>
-  </si>
-  <si>
     <t>DML777</t>
   </si>
   <si>
-    <t>Vehículos más veces registrados en un parqueadero: Parqueadero Barato XL</t>
+    <t>ZAP234</t>
+  </si>
+  <si>
+    <t>Vehículos más veces registrados en un parqueadero: Parqueadero La Tertulia</t>
   </si>
   <si>
     <t>Hoy</t>
@@ -81,22 +99,22 @@
     <t>Año</t>
   </si>
   <si>
-    <t>Ganancias de un parqueadero: Parqueadero Barato XL</t>
-  </si>
-  <si>
-    <t>Las ganancias de la fecha de hoy 2024-03-17 son: $ 6.400</t>
-  </si>
-  <si>
-    <t>Las ganancias de esta semana son: $ 6.400</t>
-  </si>
-  <si>
-    <t>Las ganancias del mes de MARCH son: $ 6.400</t>
-  </si>
-  <si>
-    <t>Las ganancias del año de 2024 son: $ 6.400</t>
-  </si>
-  <si>
-    <t>Coincidencias de la placa: D</t>
+    <t>Ganancias de un parqueadero: Parqueadero La Tertulia</t>
+  </si>
+  <si>
+    <t>Las ganancias de la fecha de hoy 2024-03-18 son: $ 0</t>
+  </si>
+  <si>
+    <t>Las ganancias de esta semana son: $ 0</t>
+  </si>
+  <si>
+    <t>Las ganancias del mes de MARCH son: $ 2.400</t>
+  </si>
+  <si>
+    <t>Las ganancias del año de 2024 son: $ 32.746</t>
+  </si>
+  <si>
+    <t>Coincidencias de la placa: DM</t>
   </si>
 </sst>
 </file>
@@ -204,7 +222,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -228,7 +246,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -239,7 +257,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>6.0</v>
+        <v>11.0</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -250,13 +268,24 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>7.0</v>
+        <v>13.0</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -269,7 +298,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -277,7 +306,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -288,83 +317,116 @@
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>2.0</v>
+        <v>30.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>4.0</v>
+        <v>29.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>7.0</v>
+        <v>12.0</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C11" s="3" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -378,7 +440,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -386,7 +448,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
@@ -397,67 +459,67 @@
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>2.0</v>
+        <v>30.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>6.0</v>
+        <v>11.0</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -471,9 +533,42 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C11" s="3" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -495,27 +590,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -533,7 +628,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
@@ -549,35 +644,35 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>9.0</v>
+        <v>33.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>10.0</v>
+        <v>35.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>11.0</v>
+        <v>36.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>